<commit_message>
update to add JSON and ClassTest to project
</commit_message>
<xml_diff>
--- a/OpenpyxlTEST/testrange.xlsx
+++ b/OpenpyxlTEST/testrange.xlsx
@@ -4,12 +4,15 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Pi" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName localSheetId="0" name="Pi">Pi!F5</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -30,18 +33,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,9 +53,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -356,7 +352,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="F5:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,20 +378,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3"/>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
+    <row r="5" spans="1:6">
+      <c r="F5" t="n">
+        <v>3.14</v>
+      </c>
     </row>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>